<commit_message>
Update to Gantt chart
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Start Date</t>
   </si>
@@ -48,15 +48,6 @@
   </si>
   <si>
     <t>Term</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Running</t>
-  </si>
-  <si>
-    <t>Extras</t>
   </si>
   <si>
     <t>Write-Up</t>
@@ -81,6 +72,12 @@
   </si>
   <si>
     <t>Writing Code</t>
+  </si>
+  <si>
+    <t>Running/Extras</t>
+  </si>
+  <si>
+    <t>Testing/Bug-Fixing</t>
   </si>
 </sst>
 </file>
@@ -249,20 +246,17 @@
                 <c:pt idx="3">
                   <c:v>Exam Revision</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Programming</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Writing Code</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Testing</c:v>
+                  <c:v>Testing/Bug-Fixing</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Running</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Extras</c:v>
+                  <c:v>Running/Extras</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Write-Up</c:v>
@@ -300,19 +294,16 @@
                 <c:pt idx="3">
                   <c:v>43562.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43499.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43499.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43538.0</c:v>
+                  <c:v>43525.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43538.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>43538.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
@@ -356,6 +347,211 @@
             <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="wdUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="wdUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="wdUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent2"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -374,20 +570,17 @@
                 <c:pt idx="3">
                   <c:v>Exam Revision</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Programming</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Writing Code</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Testing</c:v>
+                  <c:v>Testing/Bug-Fixing</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Running</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Extras</c:v>
+                  <c:v>Running/Extras</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Write-Up</c:v>
@@ -425,20 +618,17 @@
                 <c:pt idx="3">
                   <c:v>61.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>63.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>37.0</c:v>
@@ -467,7 +657,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="78"/>
+        <c:gapWidth val="41"/>
         <c:overlap val="100"/>
         <c:axId val="695637600"/>
         <c:axId val="693112064"/>
@@ -497,11 +687,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1182,16 +1372,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>135103</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>824146</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>148616</xdr:rowOff>
+      <xdr:rowOff>135105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>67551</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>94572</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>94572</xdr:rowOff>
+      <xdr:rowOff>81061</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1479,7 +1669,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1550,7 +1740,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>43562</v>
@@ -1564,87 +1754,76 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2">
-        <v>43499</v>
-      </c>
-      <c r="C6" s="2">
-        <v>43562</v>
-      </c>
-      <c r="D6">
-        <f>-(B6-C6)</f>
-        <v>63</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43499</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43562</v>
+      </c>
+      <c r="D7">
+        <f>-(B7-C7)</f>
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>43499</v>
       </c>
       <c r="C8" s="2">
-        <v>43538</v>
+        <v>43525</v>
       </c>
       <c r="D8">
         <f>-(B8-C8)</f>
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2">
+        <v>43525</v>
+      </c>
+      <c r="C9" s="2">
         <v>43538</v>
-      </c>
-      <c r="C9" s="2">
-        <v>43562</v>
       </c>
       <c r="D9">
         <f>-(B9-C9)</f>
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2">
         <v>43538</v>
       </c>
       <c r="C10" s="2">
-        <v>43539</v>
+        <v>43562</v>
       </c>
       <c r="D10">
         <f>-(B10-C10)</f>
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>43538</v>
-      </c>
-      <c r="C11" s="2">
-        <v>43539</v>
-      </c>
-      <c r="D11">
-        <f>-(B11-C11)</f>
-        <v>1</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2">
         <v>43562</v>
@@ -1659,7 +1838,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>43562</v>
@@ -1674,7 +1853,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2">
         <v>43569</v>
@@ -1689,7 +1868,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2">
         <v>43586</v>
@@ -1704,7 +1883,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>43598</v>

</xml_diff>

<commit_message>
Report work, finished Gantt chart
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -41,15 +41,6 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Easter</t>
-  </si>
-  <si>
-    <t>Exams</t>
-  </si>
-  <si>
-    <t>Term</t>
-  </si>
-  <si>
     <t>Write-Up</t>
   </si>
   <si>
@@ -78,6 +69,15 @@
   </si>
   <si>
     <t>Testing/Bug-Fixing</t>
+  </si>
+  <si>
+    <t>Exam Period</t>
+  </si>
+  <si>
+    <t>Term Time</t>
+  </si>
+  <si>
+    <t>Easter Break</t>
   </si>
 </sst>
 </file>
@@ -119,10 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -235,13 +237,13 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>Term</c:v>
+                  <c:v>Term Time</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Easter</c:v>
+                  <c:v>Easter Break</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Exams</c:v>
+                  <c:v>Exam Period</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Exam Revision</c:v>
@@ -422,6 +424,23 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="6"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
@@ -480,6 +499,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent6">
                   <a:lumMod val="75000"/>
+                  <a:alpha val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -559,13 +579,13 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>Term</c:v>
+                  <c:v>Term Time</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Easter</c:v>
+                  <c:v>Easter Break</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Exams</c:v>
+                  <c:v>Exam Period</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Exam Revision</c:v>
@@ -669,6 +689,21 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
@@ -727,8 +762,9 @@
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="15000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1373,15 +1409,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>824146</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>135105</xdr:rowOff>
+      <xdr:colOff>770103</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175638</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>94572</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>81061</xdr:rowOff>
+      <xdr:colOff>40529</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>121595</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1666,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1680,7 +1716,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1695,7 +1731,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
         <v>43499</v>
@@ -1710,7 +1746,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
         <v>43562</v>
@@ -1725,7 +1761,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>43605</v>
@@ -1740,7 +1776,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>43562</v>
@@ -1759,7 +1795,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>43499</v>
@@ -1774,7 +1810,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <v>43499</v>
@@ -1789,7 +1825,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>43525</v>
@@ -1804,7 +1840,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>43538</v>
@@ -1823,7 +1859,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2">
         <v>43562</v>
@@ -1838,7 +1874,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>43562</v>
@@ -1853,7 +1889,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2">
         <v>43569</v>
@@ -1868,7 +1904,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2">
         <v>43586</v>
@@ -1883,7 +1919,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B16" s="2">
         <v>43598</v>
@@ -1896,13 +1932,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>